<commit_message>
nova pagina só parecer final
</commit_message>
<xml_diff>
--- a/statics/MAPA_FINAL_2023_EJA.xlsx
+++ b/statics/MAPA_FINAL_2023_EJA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f28ae49758e922e1/Desktop/devbook/editabletable/statics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{DE8B4300-C710-4512-9140-032B52C9AE18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{844AA94F-CFB9-4DFB-A341-8F665D4C76B4}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{DE8B4300-C710-4512-9140-032B52C9AE18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB0582A9-0FA7-436B-BD1E-0F72307ECFB4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{BCAD9878-E9D0-420E-8A55-493979D05A8F}"/>
   </bookViews>
@@ -416,14 +416,7 @@
     <cellStyle name="20% - Ênfase3" xfId="1" builtinId="38"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFFF0066"/>
-      </font>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <b/>
@@ -433,18 +426,8 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFFF0066"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FFFF0066"/>
       </font>
     </dxf>
@@ -822,8 +805,8 @@
   <dimension ref="A1:Q131"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
+      <pane ySplit="4" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H127" sqref="H127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,7 +883,7 @@
       <c r="P3" s="22"/>
       <c r="Q3" s="22"/>
     </row>
-    <row r="4" spans="1:17" ht="186.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="162" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14"/>
       <c r="B4" s="18" t="s">
         <v>10</v>
@@ -3354,18 +3337,25 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C3"/>
   </mergeCells>
+  <conditionalFormatting sqref="B5:P130">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="notEqual">
+      <formula>"PC"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="Q5 Q8 Q11 Q14 Q17 Q20 Q23 Q26 Q29 Q32 Q35 Q38 Q41 Q44 Q47 Q50 Q53 Q56 Q59 Q62 Q65 Q68 Q71 Q74 Q77 Q80 Q83 Q86 Q89 Q92 Q95 Q98 Q101 Q104 Q107 Q110 Q113 Q116 Q119 Q122 Q125 Q128">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="lessThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5:P130">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
-      <formula>"PC"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.15748031496062992" header="0" footer="0"/>
+  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.55118110236220474" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <rowBreaks count="5" manualBreakCount="5">
+    <brk id="25" max="16383" man="1"/>
+    <brk id="46" max="16383" man="1"/>
+    <brk id="67" max="16383" man="1"/>
+    <brk id="88" max="16383" man="1"/>
+    <brk id="109" max="16383" man="1"/>
+  </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>